<commit_message>
last point unit 3 file open & save
</commit_message>
<xml_diff>
--- a/@list.xlsx
+++ b/@list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26130"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\BCA\Semester 4\C#\program\unit-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AC3C4C8-E9A2-4D41-82A1-0639D3616C6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D2FF4B2-984E-44A1-A246-2ADEA7686B0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2268" yWindow="2268" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Programs</t>
   </si>
@@ -73,6 +73,24 @@
   </si>
   <si>
     <t>TreeView Control</t>
+  </si>
+  <si>
+    <t>contextText Menu strip Control</t>
+  </si>
+  <si>
+    <t>Mdi Form With menu strip Control</t>
+  </si>
+  <si>
+    <t>Tooltip Control</t>
+  </si>
+  <si>
+    <t>Common Dialog Control</t>
+  </si>
+  <si>
+    <t>Rich Text Box Control</t>
+  </si>
+  <si>
+    <t>File Open &amp; Save</t>
   </si>
 </sst>
 </file>
@@ -396,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -528,6 +546,54 @@
         <v>15</v>
       </c>
     </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>